<commit_message>
NTD report: data preparation
</commit_message>
<xml_diff>
--- a/public/ntd_template.xlsx
+++ b/public/ntd_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11616" yWindow="-12" windowWidth="11448" windowHeight="10272"/>
+    <workbookView xWindow="11616" yWindow="-12" windowWidth="11448" windowHeight="10272" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="18" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="54">
   <si>
     <t>Unlinked passenger trips</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Passenger miles (Ops Research)</t>
   </si>
   <si>
-    <t>+/-: Special events, missed service (listed on form)</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -174,31 +171,25 @@
     <t>Unlinked Passenger Trips (UPT)</t>
   </si>
   <si>
-    <t>This number is reported by the vendor, but is also available in Para-Trapeze database.  Report number as totals for each service day type.</t>
-  </si>
-  <si>
-    <t>This will be uncommon.  Report any special activities, or disruptions to service.</t>
-  </si>
-  <si>
-    <t>This number will in all likelyhood be the same as line #8, as they are both drawn from Paratrapeze.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vendor will report this number, or else Paratrapeze can be used to derive mileage for the month.  Be sure to break out the amounts as they relate to each type of daily service run for the month. *Report totals, not averages.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vendor will report this number, or else Paratrapeze can be used to derive hours for the month.  Be sure to break out the amounts as they relate to each type of daily service run for the month. *Report totals, not averages.</t>
-  </si>
-  <si>
     <t>Passenger miles traveled (PMT)</t>
   </si>
   <si>
-    <t>This number is available in Paratrapeze.  Not normally reported by the vendor.  Report number as totals for each service day type.</t>
-  </si>
-  <si>
     <t>Periods of Service</t>
   </si>
   <si>
     <t>Actual hours less Revenue Miles +/- Special events, missed service</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>This number will in all likelyhood be the same as line #8, as they are both drawn from RidePilot.</t>
+  </si>
+  <si>
+    <t>Report number as totals for each service day type.</t>
+  </si>
+  <si>
+    <t>Report totals, not averages.</t>
   </si>
 </sst>
 </file>
@@ -212,12 +203,19 @@
     <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -514,289 +512,292 @@
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="8" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="10" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="10" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="17" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="17" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="17" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="10" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="6" borderId="2" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="23" fillId="6" borderId="2" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="2" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="8" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="17" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="8" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="9" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="9" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="17" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="17" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="17" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="9" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="6" borderId="2" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="6" borderId="2" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="2" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="17" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="8" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -1176,9 +1177,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1197,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="68" customFormat="1" ht="22.8" x14ac:dyDescent="0.2">
       <c r="A1" s="76" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="84" t="s">
         <v>5</v>
@@ -1207,15 +1208,15 @@
       <c r="F1" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="99"/>
+      <c r="G1" s="98"/>
       <c r="I1" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="K1" s="86" t="s">
         <v>42</v>
-      </c>
-      <c r="K1" s="86" t="s">
-        <v>43</v>
       </c>
       <c r="L1" s="71"/>
       <c r="M1" s="71"/>
@@ -1232,21 +1233,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="74" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="87"/>
+        <v>43</v>
+      </c>
+      <c r="D2" s="90" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="87" t="s">
+        <v>29</v>
+      </c>
       <c r="F2" s="87"/>
-      <c r="G2" s="100"/>
+      <c r="G2" s="99"/>
       <c r="H2" s="88"/>
       <c r="I2" s="87" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="87" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" s="87" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2" s="71"/>
       <c r="M2" s="71"/>
@@ -1263,21 +1268,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="74" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="89"/>
       <c r="E3" s="87"/>
       <c r="F3" s="87"/>
-      <c r="G3" s="100"/>
+      <c r="G3" s="99"/>
       <c r="H3" s="88"/>
       <c r="I3" s="87" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" s="87" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K3" s="87" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" s="71"/>
       <c r="M3" s="71"/>
@@ -1313,7 +1318,7 @@
     <row r="5" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="C5" s="50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4"/>
       <c r="F5" s="5"/>
@@ -1331,7 +1336,7 @@
     </row>
     <row r="6" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="1"/>
@@ -1347,7 +1352,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="20">
         <f>MAX(F7:Q7)</f>
@@ -1374,7 +1379,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="20">
         <f>MAX(F8:Q8)</f>
@@ -1439,7 +1444,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="20">
         <f>SUM(F11:Q11)</f>
@@ -1510,7 +1515,7 @@
     <row r="14" spans="1:20" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="53"/>
       <c r="D14" s="28">
@@ -1612,7 +1617,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="20">
         <f>SUM(F17:Q17)</f>
@@ -1681,7 +1686,7 @@
     <row r="20" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
       <c r="B20" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="53"/>
       <c r="D20" s="34">
@@ -1759,7 +1764,7 @@
     </row>
     <row r="22" spans="1:17" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="52"/>
       <c r="D22" s="8"/>
@@ -1782,7 +1787,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="52"/>
       <c r="D23" s="8"/>
@@ -1806,7 +1811,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="20">
         <f>SUM(F24:Q24)</f>
@@ -1877,7 +1882,7 @@
     <row r="27" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="52"/>
       <c r="D27" s="39">
@@ -1939,7 +1944,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="52"/>
       <c r="D28" s="28"/>
@@ -1963,7 +1968,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29" s="20">
         <f>SUM(F29:Q29)</f>
@@ -2034,7 +2039,7 @@
     <row r="32" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="91"/>
       <c r="B32" s="49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="55"/>
       <c r="D32" s="39">
@@ -2099,7 +2104,7 @@
         <v>10</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="1"/>
@@ -2111,8 +2116,8 @@
       <c r="B34" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="101" t="s">
-        <v>56</v>
+      <c r="C34" s="100" t="s">
+        <v>49</v>
       </c>
       <c r="D34" s="24">
         <f t="shared" ref="D34:D37" si="4">+D24-D29</f>
@@ -2173,7 +2178,7 @@
       <c r="B35" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="101"/>
+      <c r="C35" s="100"/>
       <c r="D35" s="24">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2233,7 +2238,7 @@
       <c r="B36" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="101"/>
+      <c r="C36" s="100"/>
       <c r="D36" s="24">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2291,9 +2296,9 @@
     <row r="37" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
       <c r="B37" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="101"/>
+        <v>14</v>
+      </c>
+      <c r="C37" s="100"/>
       <c r="D37" s="41">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2353,7 +2358,7 @@
         <v>11</v>
       </c>
       <c r="B38" s="62" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C38" s="52"/>
       <c r="D38" s="8"/>
@@ -2377,7 +2382,7 @@
         <v>8</v>
       </c>
       <c r="C39" s="54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D39" s="8">
         <f>SUM(F39:Q39)</f>
@@ -2448,7 +2453,7 @@
     <row r="42" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
       <c r="B42" s="49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C42" s="54"/>
       <c r="D42" s="28">
@@ -2534,7 +2539,7 @@
         <v>8</v>
       </c>
       <c r="C44" s="54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="8">
         <f>SUM(F44:Q44)</f>
@@ -2605,7 +2610,7 @@
     <row r="47" spans="1:17" s="46" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A47" s="45"/>
       <c r="B47" s="49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C47" s="55"/>
       <c r="D47" s="28">
@@ -2667,7 +2672,7 @@
     </row>
     <row r="48" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48" s="2"/>
       <c r="D48" s="6"/>
@@ -2688,7 +2693,7 @@
         <v>13</v>
       </c>
       <c r="B49" s="62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C49" s="56"/>
       <c r="D49" s="6"/>
@@ -2710,7 +2715,7 @@
         <v>8</v>
       </c>
       <c r="C50" s="54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D50" s="8">
         <f>SUM(F50:Q50)</f>
@@ -2781,7 +2786,7 @@
     <row r="53" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="30"/>
       <c r="B53" s="49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C53" s="57"/>
       <c r="D53" s="39">
@@ -2843,7 +2848,7 @@
         <v>14</v>
       </c>
       <c r="B54" s="63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C54" s="56"/>
       <c r="D54" s="10"/>
@@ -2858,7 +2863,7 @@
         <v>8</v>
       </c>
       <c r="C55" s="54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D55" s="8">
         <f>SUM(F55:Q55)</f>
@@ -2929,7 +2934,7 @@
     <row r="58" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="30"/>
       <c r="B58" s="49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C58" s="57"/>
       <c r="D58" s="39">
@@ -2991,7 +2996,7 @@
         <v>15</v>
       </c>
       <c r="B59" s="64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C59" s="52"/>
       <c r="E59" s="19"/>
@@ -3001,8 +3006,8 @@
       <c r="B60" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="101" t="s">
-        <v>29</v>
+      <c r="C60" s="100" t="s">
+        <v>28</v>
       </c>
       <c r="D60" s="29">
         <f t="shared" ref="D60:D62" si="13">+D50-D55</f>
@@ -3063,7 +3068,7 @@
       <c r="B61" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C61" s="101"/>
+      <c r="C61" s="100"/>
       <c r="D61" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
@@ -3123,7 +3128,7 @@
       <c r="B62" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C62" s="101"/>
+      <c r="C62" s="100"/>
       <c r="D62" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
@@ -3181,9 +3186,9 @@
     <row r="63" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="30"/>
       <c r="B63" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63" s="101"/>
+        <v>14</v>
+      </c>
+      <c r="C63" s="100"/>
       <c r="D63" s="41">
         <f>SUM(D60:D62)</f>
         <v>0</v>
@@ -3253,10 +3258,10 @@
   <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD59"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3269,7 +3274,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="77" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
@@ -3277,253 +3282,242 @@
     </row>
     <row r="3" spans="1:3" s="80" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="80" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="81" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="4" spans="1:3" s="80" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="97"/>
+      <c r="A4" s="96"/>
       <c r="C4" s="81"/>
     </row>
-    <row r="5" spans="1:3" s="95" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="95" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="96"/>
+    <row r="5" spans="1:3" s="94" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="95"/>
     </row>
     <row r="6" spans="1:3" s="93" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="98">
+      <c r="A6" s="97">
         <v>1</v>
       </c>
       <c r="B6" s="82" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="92" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="93" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="97">
+        <v>2</v>
+      </c>
+      <c r="B7" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="92" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="93" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98">
-        <v>2</v>
-      </c>
-      <c r="B7" s="82" t="s">
+      <c r="C7" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="92" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="8" spans="1:3" s="93" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="95"/>
+      <c r="A8" s="94"/>
       <c r="B8" s="82"/>
       <c r="C8" s="92"/>
     </row>
     <row r="9" spans="1:3" s="93" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="94" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="82"/>
       <c r="C9" s="92"/>
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="98">
+      <c r="A10" s="97">
         <v>3</v>
       </c>
       <c r="B10" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="79" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="98"/>
+      <c r="A11" s="97"/>
       <c r="B11" s="82"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="98">
+      <c r="A12" s="97">
         <v>4</v>
       </c>
       <c r="B12" s="82" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="98"/>
+      <c r="A13" s="97"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="98">
+      <c r="A14" s="97">
         <v>5</v>
       </c>
       <c r="B14" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="94" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="C14" s="101" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="98"/>
+      <c r="A15" s="97"/>
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="98">
+      <c r="A16" s="97">
         <v>6</v>
       </c>
       <c r="B16" s="82" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="83" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="97"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="94" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="97">
+        <v>7</v>
+      </c>
+      <c r="B19" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="101" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="97"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="97">
+        <v>8</v>
+      </c>
+      <c r="B21" s="82" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="101" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="97"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="97"/>
+      <c r="B23" s="82"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="97">
+        <v>10</v>
+      </c>
+      <c r="B24" s="82" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="79" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="98"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="95" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="98">
-        <v>7</v>
-      </c>
-      <c r="B19" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="94" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="97"/>
+      <c r="B25" s="82"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="97">
+        <v>11</v>
+      </c>
+      <c r="B26" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="101" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="98"/>
-    </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="98">
-        <v>8</v>
-      </c>
-      <c r="B21" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="94" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="98"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="98">
-        <v>9</v>
-      </c>
-      <c r="B23" s="82" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="97"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="97">
+        <v>12</v>
+      </c>
+      <c r="B28" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="102" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="97"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="97">
+        <v>13</v>
+      </c>
+      <c r="B31" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="101" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="97"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="97">
         <v>14</v>
       </c>
-      <c r="C23" s="92" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="98"/>
-      <c r="B24" s="82"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="98">
-        <v>10</v>
-      </c>
-      <c r="B25" s="82" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="79" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="98"/>
-      <c r="B26" s="82"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="98">
-        <v>11</v>
-      </c>
-      <c r="B27" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="94" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="98"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="98">
-        <v>12</v>
-      </c>
-      <c r="B29" s="82" t="s">
+      <c r="B33" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="101" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="92" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="98"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="95" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="98">
-        <v>13</v>
-      </c>
-      <c r="B32" s="82" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="94" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="98"/>
-    </row>
-    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="98">
-        <v>14</v>
-      </c>
-      <c r="B34" s="82" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="97"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="97">
+        <v>15</v>
+      </c>
+      <c r="B35" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="94" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="98"/>
+      <c r="C35" s="79" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="98">
-        <v>15</v>
-      </c>
-      <c r="B36" s="82" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="79" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="98"/>
+      <c r="A36" s="97"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update ntd template file cell formatter
</commit_message>
<xml_diff>
--- a/public/ntd_template.xlsx
+++ b/public/ntd_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xudongliu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xudongliu\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -383,7 +383,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -433,9 +433,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -445,10 +442,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
@@ -457,9 +450,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -487,10 +477,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -502,9 +488,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -534,9 +517,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -557,9 +537,6 @@
     <xf numFmtId="164" fontId="7" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -622,6 +599,61 @@
     </xf>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="8" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -953,16 +985,16 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="51" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" style="44" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.88671875" style="7" customWidth="1"/>
@@ -971,125 +1003,125 @@
     <col min="21" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="68" customFormat="1" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:20" s="59" customFormat="1" ht="22.8" x14ac:dyDescent="0.2">
+      <c r="A1" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="85"/>
-      <c r="I1" s="79" t="s">
+      <c r="G1" s="76"/>
+      <c r="I1" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="J1" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-    </row>
-    <row r="2" spans="1:20" s="68" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75">
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+    </row>
+    <row r="2" spans="1:20" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="66">
         <v>1</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="80" t="s">
+      <c r="D2" s="74"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="80" t="s">
+      <c r="J2" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="80" t="s">
+      <c r="K2" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-    </row>
-    <row r="3" spans="1:20" s="68" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75">
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+    </row>
+    <row r="3" spans="1:20" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="66">
         <v>2</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="80" t="s">
+      <c r="D3" s="73"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="80" t="s">
+      <c r="J3" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="80" t="s">
+      <c r="K3" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="71"/>
-      <c r="T3" s="71"/>
-    </row>
-    <row r="4" spans="1:20" s="68" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="70"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="71"/>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="71"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="73"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="62"/>
+      <c r="T3" s="62"/>
+    </row>
+    <row r="4" spans="1:20" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="58"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="61"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="64"/>
     </row>
     <row r="5" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="43" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="4"/>
@@ -1107,7 +1139,7 @@
       <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="7"/>
@@ -1117,64 +1149,64 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="20">
         <v>3</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="19">
         <f>MAX(F7:Q7)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="60"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
     </row>
     <row r="8" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="20">
         <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="19">
         <f>MAX(F8:Q8)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
     </row>
     <row r="9" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="13"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="19"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -1189,13 +1221,13 @@
       <c r="Q9" s="8"/>
     </row>
     <row r="10" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="20">
         <v>5</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="51"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="16"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -1211,164 +1243,164 @@
       <c r="Q10" s="8"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="41"/>
+      <c r="B11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="19">
         <f>SUM(F11:Q11)</f>
         <v>0</v>
       </c>
       <c r="E11" s="14"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="65"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="26" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="20">
+      <c r="C12" s="45"/>
+      <c r="D12" s="19">
         <f>SUM(F12:Q12)</f>
         <v>0</v>
       </c>
       <c r="E12" s="14"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="65"/>
-      <c r="O12" s="65"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="65"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="57"/>
+      <c r="Q12" s="57"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="26" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="20">
+      <c r="C13" s="45"/>
+      <c r="D13" s="19">
         <f>SUM(F13:Q13)</f>
         <v>0</v>
       </c>
       <c r="E13" s="14"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="65"/>
-      <c r="O13" s="65"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="65"/>
-    </row>
-    <row r="14" spans="1:20" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31" t="s">
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+    </row>
+    <row r="14" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="28">
+      <c r="C14" s="46"/>
+      <c r="D14" s="25">
         <f>SUM(D11:D13)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="39">
+      <c r="E14" s="36"/>
+      <c r="F14" s="35">
         <f>SUM(F11:F13)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="39">
+      <c r="G14" s="35">
         <f t="shared" ref="G14:Q14" si="0">SUM(G11:G13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="39">
+      <c r="H14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="39">
+      <c r="J14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L14" s="39">
+      <c r="L14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M14" s="39">
+      <c r="M14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N14" s="39">
+      <c r="N14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O14" s="39">
+      <c r="O14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P14" s="39">
+      <c r="P14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="39">
+      <c r="Q14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
+    <row r="15" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
     </row>
     <row r="16" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+      <c r="A16" s="20">
         <v>6</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="51"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="16"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -1384,161 +1416,161 @@
       <c r="Q16" s="8"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="26" t="s">
+      <c r="A17" s="41"/>
+      <c r="B17" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <f>SUM(F17:Q17)</f>
         <v>0</v>
       </c>
       <c r="E17" s="14"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="52"/>
-      <c r="D18" s="20">
+      <c r="C18" s="45"/>
+      <c r="D18" s="19">
         <f>SUM(F18:Q18)</f>
         <v>0</v>
       </c>
       <c r="E18" s="14"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="61"/>
-      <c r="P18" s="61"/>
-      <c r="Q18" s="61"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="53"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="53"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="52"/>
-      <c r="D19" s="20">
+      <c r="C19" s="45"/>
+      <c r="D19" s="19">
         <f>SUM(F19:Q19)</f>
         <v>0</v>
       </c>
       <c r="E19" s="14"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="61"/>
-    </row>
-    <row r="20" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31" t="s">
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="53"/>
+    </row>
+    <row r="20" spans="1:17" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="34">
+      <c r="C20" s="46"/>
+      <c r="D20" s="30">
         <f>SUM(F20:Q20)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37">
+      <c r="E20" s="32"/>
+      <c r="F20" s="33">
         <f>SUM(F17:F19)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="33">
         <f t="shared" ref="G20:Q20" si="1">+G17+G18+G19</f>
         <v>0</v>
       </c>
-      <c r="H20" s="37">
+      <c r="H20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I20" s="37">
+      <c r="I20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J20" s="37">
+      <c r="J20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K20" s="37">
+      <c r="K20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L20" s="37">
+      <c r="L20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M20" s="37">
+      <c r="M20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N20" s="37">
+      <c r="N20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="37">
+      <c r="O20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P20" s="37">
+      <c r="P20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="37">
+      <c r="Q20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="33"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
     </row>
     <row r="22" spans="1:17" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="52"/>
+      <c r="C22" s="45"/>
       <c r="D22" s="8"/>
       <c r="E22" s="12"/>
       <c r="F22" s="9"/>
@@ -1555,13 +1587,13 @@
       <c r="Q22" s="9"/>
     </row>
     <row r="23" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+      <c r="A23" s="21">
         <v>7</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="52"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="8"/>
       <c r="E23" s="12"/>
       <c r="F23" s="9"/>
@@ -1578,1439 +1610,1474 @@
       <c r="Q23" s="9"/>
     </row>
     <row r="24" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="26" t="s">
+      <c r="A24" s="22"/>
+      <c r="B24" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="16">
         <f>SUM(F24:Q24)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="59"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
     </row>
     <row r="25" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="26" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="20">
+      <c r="C25" s="45"/>
+      <c r="D25" s="16">
         <f>SUM(F25:Q25)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="59"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="79"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="79"/>
+      <c r="P25" s="79"/>
+      <c r="Q25" s="79"/>
     </row>
     <row r="26" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="26" t="s">
+      <c r="A26" s="21"/>
+      <c r="B26" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="52"/>
-      <c r="D26" s="20">
+      <c r="C26" s="45"/>
+      <c r="D26" s="16">
         <f>SUM(F26:Q26)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="59"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="79"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="79"/>
+      <c r="M26" s="79"/>
+      <c r="N26" s="79"/>
+      <c r="O26" s="79"/>
+      <c r="P26" s="79"/>
+      <c r="Q26" s="79"/>
     </row>
     <row r="27" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="31" t="s">
+      <c r="A27" s="21"/>
+      <c r="B27" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="39">
+      <c r="C27" s="45"/>
+      <c r="D27" s="81">
         <f>SUM(D24:D26)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="39">
+      <c r="E27" s="80"/>
+      <c r="F27" s="81">
         <f>SUM(F24:F26)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="39">
+      <c r="G27" s="81">
         <f t="shared" ref="G27:Q27" si="2">SUM(G24:G26)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="39">
+      <c r="H27" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I27" s="39">
+      <c r="I27" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J27" s="39">
+      <c r="J27" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K27" s="39">
+      <c r="K27" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L27" s="39">
+      <c r="L27" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M27" s="39">
+      <c r="M27" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N27" s="39">
+      <c r="N27" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O27" s="39">
+      <c r="O27" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P27" s="39">
+      <c r="P27" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q27" s="39">
+      <c r="Q27" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
+      <c r="A28" s="21">
         <v>8</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="52"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="83"/>
+      <c r="H28" s="83"/>
+      <c r="I28" s="83"/>
+      <c r="J28" s="83"/>
+      <c r="K28" s="83"/>
+      <c r="L28" s="83"/>
+      <c r="M28" s="83"/>
+      <c r="N28" s="83"/>
+      <c r="O28" s="83"/>
+      <c r="P28" s="83"/>
+      <c r="Q28" s="83"/>
     </row>
     <row r="29" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="22"/>
+      <c r="B29" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="52" t="s">
+      <c r="C29" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="16">
         <f>SUM(F29:Q29)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="59"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="79"/>
+      <c r="L29" s="79"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="79"/>
+      <c r="P29" s="79"/>
+      <c r="Q29" s="79"/>
     </row>
     <row r="30" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="26" t="s">
+      <c r="A30" s="21"/>
+      <c r="B30" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="52"/>
-      <c r="D30" s="20">
+      <c r="C30" s="45"/>
+      <c r="D30" s="16">
         <f>SUM(F30:Q30)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="59"/>
-      <c r="L30" s="59"/>
-      <c r="M30" s="59"/>
-      <c r="N30" s="59"/>
-      <c r="O30" s="59"/>
-      <c r="P30" s="59"/>
-      <c r="Q30" s="59"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="79"/>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="79"/>
     </row>
     <row r="31" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="26" t="s">
+      <c r="A31" s="21"/>
+      <c r="B31" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="52"/>
-      <c r="D31" s="20">
+      <c r="C31" s="45"/>
+      <c r="D31" s="16">
         <f>SUM(F31:Q31)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="59"/>
-      <c r="M31" s="59"/>
-      <c r="N31" s="59"/>
-      <c r="O31" s="59"/>
-      <c r="P31" s="59"/>
-      <c r="Q31" s="59"/>
-    </row>
-    <row r="32" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="84"/>
-      <c r="B32" s="49" t="s">
+      <c r="E31" s="80"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79"/>
+      <c r="N31" s="79"/>
+      <c r="O31" s="79"/>
+      <c r="P31" s="79"/>
+      <c r="Q31" s="79"/>
+    </row>
+    <row r="32" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="75"/>
+      <c r="B32" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="55"/>
-      <c r="D32" s="39">
+      <c r="C32" s="48"/>
+      <c r="D32" s="81">
         <f>SUM(D29:D31)</f>
         <v>0</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="81">
         <f t="shared" ref="E32:Q32" si="3">SUM(E29:E31)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="39">
+      <c r="F32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G32" s="39">
+      <c r="G32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H32" s="39">
+      <c r="H32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I32" s="39">
+      <c r="I32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J32" s="39">
+      <c r="J32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K32" s="39">
+      <c r="K32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L32" s="39">
+      <c r="L32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M32" s="39">
+      <c r="M32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N32" s="39">
+      <c r="N32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O32" s="39">
+      <c r="O32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P32" s="39">
+      <c r="P32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q32" s="39">
+      <c r="Q32" s="81">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="22">
+      <c r="A33" s="21">
         <v>10</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="27" t="s">
+      <c r="D33" s="84"/>
+      <c r="E33" s="85"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="86"/>
+      <c r="H33" s="86"/>
+      <c r="I33" s="86"/>
+      <c r="J33" s="86"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="86"/>
+      <c r="N33" s="86"/>
+      <c r="O33" s="86"/>
+      <c r="P33" s="86"/>
+      <c r="Q33" s="86"/>
+    </row>
+    <row r="34" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="24">
+      <c r="D34" s="87">
         <f t="shared" ref="D34:D37" si="4">+D24-D29</f>
         <v>0</v>
       </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="24">
+      <c r="E34" s="88"/>
+      <c r="F34" s="87">
         <f t="shared" ref="F34:Q34" si="5">+F24-F29</f>
         <v>0</v>
       </c>
-      <c r="G34" s="24">
+      <c r="G34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H34" s="24">
+      <c r="H34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I34" s="24">
+      <c r="I34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="24">
+      <c r="J34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K34" s="24">
+      <c r="K34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L34" s="24">
+      <c r="L34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M34" s="24">
+      <c r="M34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N34" s="24">
+      <c r="N34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O34" s="24">
+      <c r="O34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P34" s="24">
+      <c r="P34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q34" s="24">
+      <c r="Q34" s="87">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="27" t="s">
+    <row r="35" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="87"/>
-      <c r="D35" s="24">
+      <c r="C35" s="78"/>
+      <c r="D35" s="87">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="24">
+      <c r="E35" s="88"/>
+      <c r="F35" s="87">
         <f t="shared" ref="F35:Q35" si="6">+F25-F30</f>
         <v>0</v>
       </c>
-      <c r="G35" s="24">
+      <c r="G35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H35" s="24">
+      <c r="H35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I35" s="24">
+      <c r="I35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J35" s="24">
+      <c r="J35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="K35" s="24">
+      <c r="K35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L35" s="24">
+      <c r="L35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M35" s="24">
+      <c r="M35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N35" s="24">
+      <c r="N35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O35" s="24">
+      <c r="O35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P35" s="24">
+      <c r="P35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q35" s="24">
+      <c r="Q35" s="87">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="27" t="s">
+    <row r="36" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="87"/>
-      <c r="D36" s="24">
+      <c r="C36" s="78"/>
+      <c r="D36" s="87">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="24">
+      <c r="E36" s="88"/>
+      <c r="F36" s="87">
         <f t="shared" ref="F36:Q36" si="7">+F26-F31</f>
         <v>0</v>
       </c>
-      <c r="G36" s="24">
+      <c r="G36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H36" s="24">
+      <c r="H36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I36" s="24">
+      <c r="I36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J36" s="24">
+      <c r="J36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K36" s="24">
+      <c r="K36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="L36" s="24">
+      <c r="L36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M36" s="24">
+      <c r="M36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N36" s="24">
+      <c r="N36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O36" s="24">
+      <c r="O36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P36" s="24">
+      <c r="P36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q36" s="24">
+      <c r="Q36" s="87">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="31" t="s">
+    <row r="37" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="B37" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="87"/>
-      <c r="D37" s="41">
+      <c r="C37" s="78"/>
+      <c r="D37" s="89">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="42">
+      <c r="E37" s="88"/>
+      <c r="F37" s="90">
         <f t="shared" ref="F37:Q37" si="8">+F27-F32</f>
         <v>0</v>
       </c>
-      <c r="G37" s="42">
+      <c r="G37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H37" s="42">
+      <c r="H37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I37" s="42">
+      <c r="I37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J37" s="42">
+      <c r="J37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K37" s="42">
+      <c r="K37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L37" s="42">
+      <c r="L37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="M37" s="42">
+      <c r="M37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N37" s="42">
+      <c r="N37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O37" s="42">
+      <c r="O37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P37" s="42">
+      <c r="P37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Q37" s="42">
+      <c r="Q37" s="90">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22">
+      <c r="A38" s="21">
         <v>11</v>
       </c>
-      <c r="B38" s="62" t="s">
+      <c r="B38" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="52"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="91"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="83"/>
+      <c r="H38" s="83"/>
+      <c r="I38" s="83"/>
+      <c r="J38" s="83"/>
+      <c r="K38" s="83"/>
+      <c r="L38" s="83"/>
+      <c r="M38" s="83"/>
+      <c r="N38" s="83"/>
+      <c r="O38" s="83"/>
+      <c r="P38" s="83"/>
+      <c r="Q38" s="83"/>
     </row>
     <row r="39" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26" t="s">
+      <c r="A39" s="22"/>
+      <c r="B39" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="54" t="s">
+      <c r="C39" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="91">
         <f>SUM(F39:Q39)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="59"/>
-      <c r="M39" s="59"/>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="59"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="79"/>
+      <c r="J39" s="79"/>
+      <c r="K39" s="79"/>
+      <c r="L39" s="79"/>
+      <c r="M39" s="79"/>
+      <c r="N39" s="79"/>
+      <c r="O39" s="79"/>
+      <c r="P39" s="79"/>
+      <c r="Q39" s="79"/>
     </row>
     <row r="40" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="26" t="s">
+      <c r="A40" s="21"/>
+      <c r="B40" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="8">
+      <c r="C40" s="47"/>
+      <c r="D40" s="91">
         <f>SUM(F40:Q40)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="59"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="59"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="59"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="59"/>
-      <c r="Q40" s="59"/>
+      <c r="E40" s="92"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="79"/>
+      <c r="H40" s="79"/>
+      <c r="I40" s="79"/>
+      <c r="J40" s="79"/>
+      <c r="K40" s="79"/>
+      <c r="L40" s="79"/>
+      <c r="M40" s="79"/>
+      <c r="N40" s="79"/>
+      <c r="O40" s="79"/>
+      <c r="P40" s="79"/>
+      <c r="Q40" s="79"/>
     </row>
     <row r="41" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="26" t="s">
+      <c r="A41" s="21"/>
+      <c r="B41" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="54"/>
-      <c r="D41" s="8">
+      <c r="C41" s="47"/>
+      <c r="D41" s="91">
         <f>SUM(F41:Q41)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="59"/>
-      <c r="K41" s="59"/>
-      <c r="L41" s="59"/>
-      <c r="M41" s="59"/>
-      <c r="N41" s="59"/>
-      <c r="O41" s="59"/>
-      <c r="P41" s="59"/>
-      <c r="Q41" s="59"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="79"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="79"/>
+      <c r="I41" s="79"/>
+      <c r="J41" s="79"/>
+      <c r="K41" s="79"/>
+      <c r="L41" s="79"/>
+      <c r="M41" s="79"/>
+      <c r="N41" s="79"/>
+      <c r="O41" s="79"/>
+      <c r="P41" s="79"/>
+      <c r="Q41" s="79"/>
     </row>
     <row r="42" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="49" t="s">
+      <c r="A42" s="21"/>
+      <c r="B42" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="54"/>
-      <c r="D42" s="28">
+      <c r="C42" s="47"/>
+      <c r="D42" s="82">
         <f>SUM(D39:D41)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="39">
+      <c r="E42" s="92"/>
+      <c r="F42" s="81">
         <f>SUM(F39:F41)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="39">
+      <c r="G42" s="81">
         <f t="shared" ref="G42:Q42" si="9">SUM(G39:G41)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="39">
+      <c r="H42" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I42" s="39">
+      <c r="I42" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J42" s="39">
+      <c r="J42" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K42" s="39">
+      <c r="K42" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L42" s="39">
+      <c r="L42" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="M42" s="39">
+      <c r="M42" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="N42" s="39">
+      <c r="N42" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="O42" s="39">
+      <c r="O42" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="P42" s="39">
+      <c r="P42" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="39">
+      <c r="Q42" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22">
+      <c r="A43" s="21">
         <v>12</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="52"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="83"/>
+      <c r="G43" s="83"/>
+      <c r="H43" s="83"/>
+      <c r="I43" s="83"/>
+      <c r="J43" s="83"/>
+      <c r="K43" s="83"/>
+      <c r="L43" s="83"/>
+      <c r="M43" s="83"/>
+      <c r="N43" s="83"/>
+      <c r="O43" s="83"/>
+      <c r="P43" s="83"/>
+      <c r="Q43" s="83"/>
     </row>
     <row r="44" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="26" t="s">
+      <c r="A44" s="22"/>
+      <c r="B44" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="54" t="s">
+      <c r="C44" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="91">
         <f>SUM(F44:Q44)</f>
         <v>0</v>
       </c>
-      <c r="E44" s="12"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="66"/>
-      <c r="H44" s="66"/>
-      <c r="I44" s="66"/>
-      <c r="J44" s="66"/>
-      <c r="K44" s="66"/>
-      <c r="L44" s="66"/>
-      <c r="M44" s="66"/>
-      <c r="N44" s="66"/>
-      <c r="O44" s="66"/>
-      <c r="P44" s="66"/>
-      <c r="Q44" s="66"/>
+      <c r="E44" s="80"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="93"/>
+      <c r="H44" s="93"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
+      <c r="O44" s="93"/>
+      <c r="P44" s="93"/>
+      <c r="Q44" s="93"/>
     </row>
     <row r="45" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="26" t="s">
+      <c r="A45" s="21"/>
+      <c r="B45" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="54"/>
-      <c r="D45" s="8">
+      <c r="C45" s="47"/>
+      <c r="D45" s="91">
         <f>SUM(F45:Q45)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="12"/>
-      <c r="F45" s="66"/>
-      <c r="G45" s="66"/>
-      <c r="H45" s="66"/>
-      <c r="I45" s="66"/>
-      <c r="J45" s="66"/>
-      <c r="K45" s="66"/>
-      <c r="L45" s="66"/>
-      <c r="M45" s="66"/>
-      <c r="N45" s="66"/>
-      <c r="O45" s="66"/>
-      <c r="P45" s="66"/>
-      <c r="Q45" s="66"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="93"/>
+      <c r="G45" s="93"/>
+      <c r="H45" s="93"/>
+      <c r="I45" s="93"/>
+      <c r="J45" s="93"/>
+      <c r="K45" s="93"/>
+      <c r="L45" s="93"/>
+      <c r="M45" s="93"/>
+      <c r="N45" s="93"/>
+      <c r="O45" s="93"/>
+      <c r="P45" s="93"/>
+      <c r="Q45" s="93"/>
     </row>
     <row r="46" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="26" t="s">
+      <c r="A46" s="21"/>
+      <c r="B46" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="54"/>
-      <c r="D46" s="8">
+      <c r="C46" s="47"/>
+      <c r="D46" s="91">
         <f>SUM(F46:Q46)</f>
         <v>0</v>
       </c>
-      <c r="E46" s="12"/>
-      <c r="F46" s="66"/>
-      <c r="G46" s="66"/>
-      <c r="H46" s="66"/>
-      <c r="I46" s="66"/>
-      <c r="J46" s="66"/>
-      <c r="K46" s="66"/>
-      <c r="L46" s="66"/>
-      <c r="M46" s="66"/>
-      <c r="N46" s="66"/>
-      <c r="O46" s="66"/>
-      <c r="P46" s="66"/>
-      <c r="Q46" s="66"/>
-    </row>
-    <row r="47" spans="1:17" s="46" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
-      <c r="A47" s="45"/>
-      <c r="B47" s="49" t="s">
+      <c r="E46" s="80"/>
+      <c r="F46" s="93"/>
+      <c r="G46" s="93"/>
+      <c r="H46" s="93"/>
+      <c r="I46" s="93"/>
+      <c r="J46" s="93"/>
+      <c r="K46" s="93"/>
+      <c r="L46" s="93"/>
+      <c r="M46" s="93"/>
+      <c r="N46" s="93"/>
+      <c r="O46" s="93"/>
+      <c r="P46" s="93"/>
+      <c r="Q46" s="93"/>
+    </row>
+    <row r="47" spans="1:17" s="40" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+      <c r="A47" s="39"/>
+      <c r="B47" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="55"/>
-      <c r="D47" s="28">
+      <c r="C47" s="48"/>
+      <c r="D47" s="82">
         <f>SUM(D44:D46)</f>
         <v>0</v>
       </c>
-      <c r="E47" s="28">
+      <c r="E47" s="82">
         <f t="shared" ref="E47:Q47" si="10">SUM(E44:E46)</f>
         <v>0</v>
       </c>
-      <c r="F47" s="28">
+      <c r="F47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G47" s="28">
+      <c r="G47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H47" s="28">
+      <c r="H47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="I47" s="28">
+      <c r="I47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J47" s="28">
+      <c r="J47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="K47" s="28">
+      <c r="K47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="L47" s="28">
+      <c r="L47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M47" s="28">
+      <c r="M47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N47" s="28">
+      <c r="N47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O47" s="28">
+      <c r="O47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P47" s="28">
+      <c r="P47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q47" s="28">
+      <c r="Q47" s="82">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="44" t="s">
+      <c r="A48" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B48" s="2"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="2"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7"/>
-      <c r="P48" s="7"/>
-      <c r="Q48" s="7"/>
+      <c r="D48" s="94"/>
+      <c r="E48" s="95"/>
+      <c r="F48" s="84"/>
+      <c r="G48" s="84"/>
+      <c r="H48" s="84"/>
+      <c r="I48" s="84"/>
+      <c r="J48" s="84"/>
+      <c r="K48" s="84"/>
+      <c r="L48" s="84"/>
+      <c r="M48" s="84"/>
+      <c r="N48" s="84"/>
+      <c r="O48" s="84"/>
+      <c r="P48" s="84"/>
+      <c r="Q48" s="84"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" s="21">
+      <c r="A49" s="20">
         <v>13</v>
       </c>
-      <c r="B49" s="62" t="s">
+      <c r="B49" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="56"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="2"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="7"/>
-      <c r="P49" s="7"/>
-      <c r="Q49" s="7"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="94"/>
+      <c r="E49" s="95"/>
+      <c r="F49" s="84"/>
+      <c r="G49" s="84"/>
+      <c r="H49" s="84"/>
+      <c r="I49" s="84"/>
+      <c r="J49" s="84"/>
+      <c r="K49" s="84"/>
+      <c r="L49" s="84"/>
+      <c r="M49" s="84"/>
+      <c r="N49" s="84"/>
+      <c r="O49" s="84"/>
+      <c r="P49" s="84"/>
+      <c r="Q49" s="84"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
-      <c r="B50" s="26" t="s">
+      <c r="A50" s="20"/>
+      <c r="B50" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="54" t="s">
+      <c r="C50" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="8">
+      <c r="D50" s="91">
         <f>SUM(F50:Q50)</f>
         <v>0</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="60"/>
-      <c r="G50" s="60"/>
-      <c r="H50" s="60"/>
-      <c r="I50" s="60"/>
-      <c r="J50" s="60"/>
-      <c r="K50" s="60"/>
-      <c r="L50" s="60"/>
-      <c r="M50" s="60"/>
-      <c r="N50" s="60"/>
-      <c r="O50" s="60"/>
-      <c r="P50" s="60"/>
-      <c r="Q50" s="60"/>
+      <c r="E50" s="95"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="96"/>
+      <c r="H50" s="96"/>
+      <c r="I50" s="96"/>
+      <c r="J50" s="96"/>
+      <c r="K50" s="96"/>
+      <c r="L50" s="96"/>
+      <c r="M50" s="96"/>
+      <c r="N50" s="96"/>
+      <c r="O50" s="96"/>
+      <c r="P50" s="96"/>
+      <c r="Q50" s="96"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="21"/>
-      <c r="B51" s="26" t="s">
+      <c r="A51" s="20"/>
+      <c r="B51" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="54"/>
-      <c r="D51" s="8">
+      <c r="C51" s="47"/>
+      <c r="D51" s="91">
         <f>SUM(F51:Q51)</f>
         <v>0</v>
       </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="60"/>
-      <c r="G51" s="60"/>
-      <c r="H51" s="60"/>
-      <c r="I51" s="60"/>
-      <c r="J51" s="60"/>
-      <c r="K51" s="60"/>
-      <c r="L51" s="60"/>
-      <c r="M51" s="60"/>
-      <c r="N51" s="60"/>
-      <c r="O51" s="60"/>
-      <c r="P51" s="60"/>
-      <c r="Q51" s="60"/>
+      <c r="E51" s="95"/>
+      <c r="F51" s="96"/>
+      <c r="G51" s="96"/>
+      <c r="H51" s="96"/>
+      <c r="I51" s="96"/>
+      <c r="J51" s="96"/>
+      <c r="K51" s="96"/>
+      <c r="L51" s="96"/>
+      <c r="M51" s="96"/>
+      <c r="N51" s="96"/>
+      <c r="O51" s="96"/>
+      <c r="P51" s="96"/>
+      <c r="Q51" s="96"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="26" t="s">
+      <c r="A52" s="20"/>
+      <c r="B52" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="54"/>
-      <c r="D52" s="8">
+      <c r="C52" s="47"/>
+      <c r="D52" s="91">
         <f>SUM(F52:Q52)</f>
         <v>0</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="60"/>
-      <c r="G52" s="60"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="60"/>
-      <c r="J52" s="60"/>
-      <c r="K52" s="60"/>
-      <c r="L52" s="60"/>
-      <c r="M52" s="60"/>
-      <c r="N52" s="60"/>
-      <c r="O52" s="60"/>
-      <c r="P52" s="60"/>
-      <c r="Q52" s="60"/>
-    </row>
-    <row r="53" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
-      <c r="B53" s="49" t="s">
+      <c r="E52" s="95"/>
+      <c r="F52" s="96"/>
+      <c r="G52" s="96"/>
+      <c r="H52" s="96"/>
+      <c r="I52" s="96"/>
+      <c r="J52" s="96"/>
+      <c r="K52" s="96"/>
+      <c r="L52" s="96"/>
+      <c r="M52" s="96"/>
+      <c r="N52" s="96"/>
+      <c r="O52" s="96"/>
+      <c r="P52" s="96"/>
+      <c r="Q52" s="96"/>
+    </row>
+    <row r="53" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="26"/>
+      <c r="B53" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="57"/>
-      <c r="D53" s="39">
+      <c r="C53" s="50"/>
+      <c r="D53" s="81">
         <f>SUM(D50:D52)</f>
         <v>0</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="39">
+      <c r="E53" s="95"/>
+      <c r="F53" s="81">
         <f>SUM(F50:F52)</f>
         <v>0</v>
       </c>
-      <c r="G53" s="39">
+      <c r="G53" s="81">
         <f t="shared" ref="G53:Q53" si="11">SUM(G50:G52)</f>
         <v>0</v>
       </c>
-      <c r="H53" s="39">
+      <c r="H53" s="81">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="I53" s="39">
+      <c r="I53" s="81">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J53" s="39">
+      <c r="J53" s="81">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K53" s="39">
+      <c r="K53" s="81">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="L53" s="39">
+      <c r="L53" s="81">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M53" s="39">
+      <c r="M53" s="81">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N53" s="39">
+      <c r="N53" s="81">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="O53" s="39">
+      <c r="O53" s="81">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P53" s="39">
+      <c r="P53" s="81">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Q53" s="39">
+      <c r="Q53" s="81">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" s="21">
+      <c r="A54" s="20">
         <v>14</v>
       </c>
-      <c r="B54" s="63" t="s">
+      <c r="B54" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="56"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="86"/>
+      <c r="E54" s="95"/>
+      <c r="F54" s="86"/>
+      <c r="G54" s="86"/>
+      <c r="H54" s="86"/>
+      <c r="I54" s="86"/>
+      <c r="J54" s="86"/>
+      <c r="K54" s="86"/>
+      <c r="L54" s="86"/>
+      <c r="M54" s="86"/>
+      <c r="N54" s="86"/>
+      <c r="O54" s="86"/>
+      <c r="P54" s="86"/>
+      <c r="Q54" s="86"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
-      <c r="B55" s="26" t="s">
+      <c r="A55" s="20"/>
+      <c r="B55" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="54" t="s">
+      <c r="C55" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D55" s="91">
         <f>SUM(F55:Q55)</f>
         <v>0</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="60"/>
-      <c r="G55" s="60"/>
-      <c r="H55" s="60"/>
-      <c r="I55" s="60"/>
-      <c r="J55" s="60"/>
-      <c r="K55" s="60"/>
-      <c r="L55" s="60"/>
-      <c r="M55" s="60"/>
-      <c r="N55" s="60"/>
-      <c r="O55" s="60"/>
-      <c r="P55" s="60"/>
-      <c r="Q55" s="60"/>
+      <c r="E55" s="95"/>
+      <c r="F55" s="96"/>
+      <c r="G55" s="96"/>
+      <c r="H55" s="96"/>
+      <c r="I55" s="96"/>
+      <c r="J55" s="96"/>
+      <c r="K55" s="96"/>
+      <c r="L55" s="96"/>
+      <c r="M55" s="96"/>
+      <c r="N55" s="96"/>
+      <c r="O55" s="96"/>
+      <c r="P55" s="96"/>
+      <c r="Q55" s="96"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56" s="21"/>
-      <c r="B56" s="26" t="s">
+      <c r="A56" s="20"/>
+      <c r="B56" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="56"/>
-      <c r="D56" s="8">
+      <c r="C56" s="49"/>
+      <c r="D56" s="91">
         <f>SUM(F56:Q56)</f>
         <v>0</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="60"/>
-      <c r="G56" s="60"/>
-      <c r="H56" s="60"/>
-      <c r="I56" s="60"/>
-      <c r="J56" s="60"/>
-      <c r="K56" s="60"/>
-      <c r="L56" s="60"/>
-      <c r="M56" s="60"/>
-      <c r="N56" s="60"/>
-      <c r="O56" s="60"/>
-      <c r="P56" s="60"/>
-      <c r="Q56" s="60"/>
+      <c r="E56" s="95"/>
+      <c r="F56" s="96"/>
+      <c r="G56" s="96"/>
+      <c r="H56" s="96"/>
+      <c r="I56" s="96"/>
+      <c r="J56" s="96"/>
+      <c r="K56" s="96"/>
+      <c r="L56" s="96"/>
+      <c r="M56" s="96"/>
+      <c r="N56" s="96"/>
+      <c r="O56" s="96"/>
+      <c r="P56" s="96"/>
+      <c r="Q56" s="96"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
-      <c r="B57" s="26" t="s">
+      <c r="A57" s="20"/>
+      <c r="B57" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="56"/>
-      <c r="D57" s="8">
+      <c r="C57" s="49"/>
+      <c r="D57" s="91">
         <f>SUM(F57:Q57)</f>
         <v>0</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="60"/>
-      <c r="G57" s="60"/>
-      <c r="H57" s="60"/>
-      <c r="I57" s="60"/>
-      <c r="J57" s="60"/>
-      <c r="K57" s="60"/>
-      <c r="L57" s="60"/>
-      <c r="M57" s="60"/>
-      <c r="N57" s="60"/>
-      <c r="O57" s="60"/>
-      <c r="P57" s="60"/>
-      <c r="Q57" s="60"/>
-    </row>
-    <row r="58" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="30"/>
-      <c r="B58" s="49" t="s">
+      <c r="E57" s="95"/>
+      <c r="F57" s="96"/>
+      <c r="G57" s="96"/>
+      <c r="H57" s="96"/>
+      <c r="I57" s="96"/>
+      <c r="J57" s="96"/>
+      <c r="K57" s="96"/>
+      <c r="L57" s="96"/>
+      <c r="M57" s="96"/>
+      <c r="N57" s="96"/>
+      <c r="O57" s="96"/>
+      <c r="P57" s="96"/>
+      <c r="Q57" s="96"/>
+    </row>
+    <row r="58" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="26"/>
+      <c r="B58" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="57"/>
-      <c r="D58" s="39">
+      <c r="C58" s="50"/>
+      <c r="D58" s="81">
         <f>SUM(D55:D57)</f>
         <v>0</v>
       </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="39">
+      <c r="E58" s="95"/>
+      <c r="F58" s="81">
         <f t="shared" ref="F58:Q58" si="12">SUM(F55:F57)</f>
         <v>0</v>
       </c>
-      <c r="G58" s="39">
+      <c r="G58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="H58" s="39">
+      <c r="H58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="I58" s="39">
+      <c r="I58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="J58" s="39">
+      <c r="J58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K58" s="39">
+      <c r="K58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="L58" s="39">
+      <c r="L58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="M58" s="39">
+      <c r="M58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="N58" s="39">
+      <c r="N58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="O58" s="39">
+      <c r="O58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P58" s="39">
+      <c r="P58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Q58" s="39">
+      <c r="Q58" s="81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22">
+    <row r="59" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="21">
         <v>15</v>
       </c>
-      <c r="B59" s="64" t="s">
+      <c r="B59" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="52"/>
-      <c r="E59" s="19"/>
-    </row>
-    <row r="60" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
-      <c r="B60" s="27" t="s">
+      <c r="C59" s="45"/>
+      <c r="D59" s="97"/>
+      <c r="E59" s="98"/>
+      <c r="F59" s="97"/>
+      <c r="G59" s="97"/>
+      <c r="H59" s="97"/>
+      <c r="I59" s="97"/>
+      <c r="J59" s="97"/>
+      <c r="K59" s="97"/>
+      <c r="L59" s="97"/>
+      <c r="M59" s="97"/>
+      <c r="N59" s="97"/>
+      <c r="O59" s="97"/>
+      <c r="P59" s="97"/>
+      <c r="Q59" s="97"/>
+    </row>
+    <row r="60" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="20"/>
+      <c r="B60" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="87" t="s">
+      <c r="C60" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="D60" s="29">
+      <c r="D60" s="99">
         <f t="shared" ref="D60:D62" si="13">+D50-D55</f>
         <v>0</v>
       </c>
-      <c r="E60" s="19"/>
-      <c r="F60" s="29">
+      <c r="E60" s="98"/>
+      <c r="F60" s="99">
         <f t="shared" ref="F60:Q60" si="14">+F50-F55</f>
         <v>0</v>
       </c>
-      <c r="G60" s="29">
+      <c r="G60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="H60" s="29">
+      <c r="H60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="I60" s="29">
+      <c r="I60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="J60" s="29">
+      <c r="J60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="K60" s="29">
+      <c r="K60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="L60" s="29">
+      <c r="L60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M60" s="29">
+      <c r="M60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="N60" s="29">
+      <c r="N60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="O60" s="29">
+      <c r="O60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="P60" s="29">
+      <c r="P60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="Q60" s="29">
+      <c r="Q60" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="21"/>
-      <c r="B61" s="27" t="s">
+    <row r="61" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="20"/>
+      <c r="B61" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C61" s="87"/>
-      <c r="D61" s="29">
+      <c r="C61" s="78"/>
+      <c r="D61" s="99">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="E61" s="19"/>
-      <c r="F61" s="29">
+      <c r="E61" s="98"/>
+      <c r="F61" s="99">
         <f t="shared" ref="F61:Q61" si="15">+F51-F56</f>
         <v>0</v>
       </c>
-      <c r="G61" s="29">
+      <c r="G61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="H61" s="29">
+      <c r="H61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="I61" s="29">
+      <c r="I61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J61" s="29">
+      <c r="J61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="K61" s="29">
+      <c r="K61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="L61" s="29">
+      <c r="L61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="M61" s="29">
+      <c r="M61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="N61" s="29">
+      <c r="N61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O61" s="29">
+      <c r="O61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="P61" s="29">
+      <c r="P61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="Q61" s="29">
+      <c r="Q61" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="21"/>
-      <c r="B62" s="27" t="s">
+    <row r="62" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="20"/>
+      <c r="B62" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="87"/>
-      <c r="D62" s="29">
+      <c r="C62" s="78"/>
+      <c r="D62" s="99">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="E62" s="19"/>
-      <c r="F62" s="29">
+      <c r="E62" s="98"/>
+      <c r="F62" s="99">
         <f t="shared" ref="F62:Q62" si="16">+F52-F57</f>
         <v>0</v>
       </c>
-      <c r="G62" s="29">
+      <c r="G62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="H62" s="29">
+      <c r="H62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I62" s="29">
+      <c r="I62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J62" s="29">
+      <c r="J62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="K62" s="29">
+      <c r="K62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="L62" s="29">
+      <c r="L62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="M62" s="29">
+      <c r="M62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N62" s="29">
+      <c r="N62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="O62" s="29">
+      <c r="O62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="P62" s="29">
+      <c r="P62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="Q62" s="29">
+      <c r="Q62" s="99">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
-      <c r="B63" s="31" t="s">
+    <row r="63" spans="1:17" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="26"/>
+      <c r="B63" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="87"/>
-      <c r="D63" s="41">
+      <c r="C63" s="78"/>
+      <c r="D63" s="89">
         <f>SUM(D60:D62)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="48"/>
-      <c r="F63" s="42">
+      <c r="E63" s="100"/>
+      <c r="F63" s="90">
         <f t="shared" ref="F63:Q63" si="17">SUM(F60:F62)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="42">
+      <c r="G63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="H63" s="42">
+      <c r="H63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="I63" s="42">
+      <c r="I63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="J63" s="42">
+      <c r="J63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="K63" s="42">
+      <c r="K63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="L63" s="42">
+      <c r="L63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="M63" s="42">
+      <c r="M63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="N63" s="42">
+      <c r="N63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="O63" s="42">
+      <c r="O63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="P63" s="42">
+      <c r="P63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="Q63" s="42">
+      <c r="Q63" s="90">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>

</xml_diff>